<commit_message>
Budget update - Resistor was added
</commit_message>
<xml_diff>
--- a/VAC Prelim 2.0/Chapter-4/tables/AcceleratedCorrosion_db075.xlsx
+++ b/VAC Prelim 2.0/Chapter-4/tables/AcceleratedCorrosion_db075.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ConditionDependentPBEE\Thesis\VAC Prelim 2.0\Chapter-4\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ConditionDepedentPBEE\Thesis\VAC Prelim 2.0\Chapter-4\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D9A7E1-33C7-43B8-9D18-5A90BED029AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Budget" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Corrosion Level</t>
   </si>
@@ -271,11 +274,20 @@
   <si>
     <t>45 Gal to</t>
   </si>
+  <si>
+    <t>Resistor 3kOhms</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Vishay-Dale/CMF073K0000JNEK?qs=w0S%252B%2FsJ%252B%2Fi0GZ3fUT3Vt%252BQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/%EF%BC%88Precision-00-01V%EF%BC%8C0-001A%EF%BC%894-Digital-Precision-Adjustable-Regulated/dp/B07M6JJS93</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -366,14 +378,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -394,23 +406,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:F14" totalsRowShown="0">
-  <autoFilter ref="A9:F14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A9:F14" totalsRowShown="0">
+  <autoFilter ref="A9:F14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Corrosion Level"/>
-    <tableColumn id="2" name="mloss">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Corrosion Level"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="mloss">
       <calculatedColumnFormula>0.25*PI()*$B$5^2*$B$6*A10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Current (A)">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Current (A)">
       <calculatedColumnFormula>+C9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Current Density (μa/cm^2)">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Current Density (μa/cm^2)">
       <calculatedColumnFormula>+C10*1000000/$B$7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="t(h)">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="t(h)">
       <calculatedColumnFormula>+(B10*$B$4*$B$3)/(C10*$B$2*60*60)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="t(days)">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="t(days)">
       <calculatedColumnFormula>+E10/24</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -680,22 +692,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="A21:C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.83984375" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.41796875" customWidth="1"/>
+    <col min="6" max="6" width="9.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -707,7 +719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -718,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -729,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -737,7 +749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -749,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -760,7 +772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -772,7 +784,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -792,7 +804,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0.05</v>
       </c>
@@ -816,7 +828,7 @@
         <v>8.9555312476121056</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>0.1</v>
       </c>
@@ -841,7 +853,7 @@
         <v>17.911062495224211</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0.15</v>
       </c>
@@ -866,7 +878,7 @@
         <v>26.866593742836319</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>0.2</v>
       </c>
@@ -891,7 +903,7 @@
         <v>35.822124990448422</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0.25</v>
       </c>
@@ -926,22 +938,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="3" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -964,7 +976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>1</v>
       </c>
@@ -977,10 +989,10 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>24.97</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <f>+E4*C4</f>
         <v>24.97</v>
       </c>
@@ -988,47 +1000,47 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>16.68</v>
       </c>
-      <c r="F5" s="9">
-        <f t="shared" ref="F5:F17" si="0">+E5*C5</f>
+      <c r="F5" s="8">
+        <f t="shared" ref="F5:F18" si="0">+E5*C5</f>
         <v>33.36</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>151.74</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>151.74</v>
       </c>
@@ -1036,23 +1048,23 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>10.89</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>130.68</v>
       </c>
@@ -1060,23 +1072,23 @@
         <v>205881703</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>24.45</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>24.45</v>
       </c>
@@ -1084,23 +1096,23 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>39.99</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>279.93</v>
       </c>
@@ -1111,23 +1123,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>10.63</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>21.26</v>
       </c>
@@ -1135,375 +1147,402 @@
         <v>295096</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>3.52</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>190.08</v>
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>79.98</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>79.98</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="8">
+        <v>8.41</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>8.41</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E14" s="8">
         <v>4.8</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F14" s="8">
         <f t="shared" si="0"/>
         <v>9.6</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="9">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E15" s="8">
         <v>53.5</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F15" s="8">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C16" s="9">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E16" s="8">
         <v>27.75</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F16" s="8">
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C17" s="9">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E17" s="8">
         <v>26.75</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>133.75</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C18" s="9">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E18" s="8">
         <v>7.5</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F18" s="8">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="11">
-        <f>SUM(F4:F17)</f>
-        <v>1305.3000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="10">
+        <f>SUM(F4:F18)</f>
+        <v>1313.71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
         <v>33</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>34</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>35</v>
       </c>
-      <c r="F20">
-        <f>+C20*3.78541</f>
+      <c r="F21">
+        <f>+C21*3.78541</f>
         <v>170.34345000000002</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>36</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <f>250/1000</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="1">
-        <f>11.22*F20</f>
-        <v>1911.2535090000003</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
       </c>
       <c r="E22">
-        <f>+C22/500</f>
-        <v>3.8225070180000005</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
-        <f>13.77*F20</f>
-        <v>2345.6293065</v>
+        <f>11.22*F21</f>
+        <v>1911.2535090000003</v>
       </c>
       <c r="D23" t="s">
         <v>37</v>
       </c>
       <c r="E23">
         <f>+C23/500</f>
-        <v>4.6912586129999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.8225070180000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1">
-        <v>150</v>
+        <f>13.77*F21</f>
+        <v>2345.6293065</v>
       </c>
       <c r="D24" t="s">
         <v>37</v>
       </c>
       <c r="E24">
-        <f>POWER(0.0000065/4,1/3)*F20*74</f>
+        <f>+C24/500</f>
+        <v>4.6912586129999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1">
+        <v>150</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <f>POWER(0.0000065/4,1/3)*F21*74</f>
         <v>148.19775124007987</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
         <v>54</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>0.75</v>
-      </c>
-      <c r="D27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28">
-        <v>17.5</v>
       </c>
       <c r="D28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>17.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="C29">
-        <f>0.25*PI()*C27^2</f>
+      <c r="C30">
+        <f>0.25*PI()*C28^2</f>
         <v>0.44178646691106466</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
         <v>58</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <f>0.000001</f>
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31">
-        <f>+C30*C28/C29</f>
-        <v>3.9611896947316168E-5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
         <v>59</v>
       </c>
       <c r="C32">
-        <f>+C31*4</f>
+        <f>+C31*C29/C30</f>
+        <v>3.9611896947316168E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33">
+        <f>+C32*4</f>
         <v>1.5844758778926467E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
         <v>60</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
         <v>62</v>
       </c>
-      <c r="C34">
-        <f>+C33*C32</f>
+      <c r="C35">
+        <f>+C34*C33</f>
         <v>7.9223793894632341E-7</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C37">
-        <f>0.3*F20</f>
+      <c r="C38">
+        <f>0.3*F21</f>
         <v>51.103035000000006</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="G9" r:id="rId2"/>
-    <hyperlink ref="H9" r:id="rId3"/>
-    <hyperlink ref="G6" r:id="rId4"/>
-    <hyperlink ref="G4" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G13" r:id="rId7" xr:uid="{A545CD6B-43C2-4920-A5A4-DE60917CC9BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>